<commit_message>
update FE, BE after deployment
</commit_message>
<xml_diff>
--- a/api/wwwroot/Template/IMPORT_PRODUCT_TEMPLATE.xlsx
+++ b/api/wwwroot/Template/IMPORT_PRODUCT_TEMPLATE.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BXT\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BXT\Desktop\quanlykho\api\var\www\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B969D00F-1232-47A2-BE00-BA817312F022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC67B98-1C07-4222-A53D-794A51C5B607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -480,7 +480,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>